<commit_message>
[#7jt5vk] - Added statements to word and DFID download format
</commit_message>
<xml_diff>
--- a/src/main/resources/DFID_Template.xlsx
+++ b/src/main/resources/DFID_Template.xlsx
@@ -94,7 +94,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,13 +154,6 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -253,7 +246,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -282,8 +275,8 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -314,10 +307,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,35 +315,31 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -391,34 +376,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="8" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="27" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -438,27 +424,27 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -478,15 +464,15 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -506,19 +492,19 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -538,15 +524,15 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -566,27 +552,27 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D6" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -606,15 +592,15 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="15"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -634,17 +620,17 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -664,15 +650,15 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -692,27 +678,27 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D10" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -732,15 +718,15 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18"/>
-      <c r="C11" s="16"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -760,17 +746,17 @@
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="12" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -790,15 +776,15 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -818,27 +804,27 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
-      <c r="AA13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C14" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D14" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -858,15 +844,15 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="C15" s="16"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -886,17 +872,17 @@
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="12" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -916,15 +902,15 @@
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -944,27 +930,27 @@
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>13</v>
       </c>
+      <c r="C18" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D18" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -984,15 +970,15 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -1012,17 +998,17 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="12" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1042,15 +1028,15 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -1070,27 +1056,27 @@
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>13</v>
       </c>
+      <c r="C22" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D22" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -1110,15 +1096,15 @@
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -1138,19 +1124,19 @@
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="12" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1170,15 +1156,15 @@
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -1198,7 +1184,6 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2148,29 +2133,29 @@
     <row r="971" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0" footer="0"/>
@@ -2205,84 +2190,84 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
[#ayynmx] - Download statements without indicators associated to them
</commit_message>
<xml_diff>
--- a/src/main/resources/DFID_Template.xlsx
+++ b/src/main/resources/DFID_Template.xlsx
@@ -41,7 +41,7 @@
     <t xml:space="preserve">Milestone 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Milestone 3</t>
+    <t xml:space="preserve">Target</t>
   </si>
   <si>
     <t xml:space="preserve">PRIMARY THEME</t>
@@ -379,7 +379,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>